<commit_message>
users and companies script
</commit_message>
<xml_diff>
--- a/com.consero.project/src/test/resources/testdata/credential.xlsx
+++ b/com.consero.project/src/test/resources/testdata/credential.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22827"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{0F1A6E57-3853-4E8A-98E0-0118E9BA42F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="10200" windowHeight="11436" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15705" windowHeight="1950"/>
   </bookViews>
   <sheets>
     <sheet name="credentials" sheetId="1" r:id="rId1"/>
@@ -54,7 +53,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -426,22 +425,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" customWidth="1"/>
-    <col min="2" max="2" width="27.109375" customWidth="1"/>
-    <col min="3" max="3" width="20.44140625" customWidth="1"/>
-    <col min="4" max="4" width="24.109375" customWidth="1"/>
+    <col min="1" max="1" width="23.28515625" customWidth="1"/>
+    <col min="2" max="2" width="27.140625" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -455,7 +454,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -469,7 +468,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -485,8 +484,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B3" r:id="rId2" display="mailto:tmanager2@yopmail.com" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2" display="mailto:tmanager2@yopmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
profile setting and IFR script
</commit_message>
<xml_diff>
--- a/com.consero.project/src/test/resources/testdata/credential.xlsx
+++ b/com.consero.project/src/test/resources/testdata/credential.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14475" windowHeight="1980"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14130" windowHeight="8250"/>
   </bookViews>
   <sheets>
     <sheet name="credentials" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>username</t>
   </si>
@@ -57,6 +57,18 @@
   </si>
   <si>
     <t>Sowmya Boddu</t>
+  </si>
+  <si>
+    <t>profileSettings</t>
+  </si>
+  <si>
+    <t>automation+1@thinkbridge.in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neha Automation </t>
+  </si>
+  <si>
+    <t>Consero234$</t>
   </si>
 </sst>
 </file>
@@ -428,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,13 +510,28 @@
         <v>8</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
     <hyperlink ref="B3" r:id="rId2"/>
     <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>